<commit_message>
work on added text processing.
Re-generated spreadsheets in nlp, and added new spreadsheets in output to push to tableau. In notebook, found ways to extract info on the level of goods, i.e. this good was traded on these dates at a place that has a local ID of x. This has proved very useful for visualization.
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -58,24 +58,24 @@
     <t>гарусный товар</t>
   </si>
   <si>
+    <t>особливый товар</t>
+  </si>
+  <si>
     <t>мелочь</t>
   </si>
   <si>
-    <t>особливый товар</t>
+    <t>серебреный товар</t>
   </si>
   <si>
     <t>деревенский товар</t>
   </si>
   <si>
-    <t>серебреный товар</t>
+    <t>небогатый товар</t>
   </si>
   <si>
     <t>крамными товар</t>
   </si>
   <si>
-    <t>небогатый товар</t>
-  </si>
-  <si>
     <t>мясо</t>
   </si>
   <si>
@@ -85,71 +85,71 @@
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>пушной товар</t>
+  </si>
+  <si>
+    <t>нужный товар</t>
+  </si>
+  <si>
     <t>набойчатый товар</t>
   </si>
   <si>
     <t>щепетильный товар</t>
   </si>
   <si>
-    <t>пушной товар</t>
-  </si>
-  <si>
-    <t>нужный товар</t>
+    <t>медный товар</t>
+  </si>
+  <si>
+    <t>питейный припасы</t>
   </si>
   <si>
     <t>внутренний товар</t>
   </si>
   <si>
-    <t>питейный припасы</t>
-  </si>
-  <si>
     <t>недорогой товар</t>
   </si>
   <si>
-    <t>медный товар</t>
-  </si>
-  <si>
     <t>привозный товар</t>
   </si>
   <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
     <t>оловянный товар</t>
   </si>
   <si>
-    <t>суровский товар</t>
-  </si>
-  <si>
     <t>произрастание</t>
   </si>
   <si>
     <t>галантерейный товар</t>
   </si>
   <si>
+    <t>заморский товар</t>
+  </si>
+  <si>
     <t>купецкий товар</t>
   </si>
   <si>
-    <t>заморский товар</t>
-  </si>
-  <si>
     <t>меховой товар</t>
   </si>
   <si>
+    <t>рукодельный товар</t>
+  </si>
+  <si>
+    <t>домовый товар</t>
+  </si>
+  <si>
+    <t>надлежащий товар</t>
+  </si>
+  <si>
     <t>харчевой припасы</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>домовый товар</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,424 +213,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Counts</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
-              <c:strCache>
-                <c:ptCount val="42"/>
-                <c:pt idx="0">
-                  <c:v>мелочный товар</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>шелковый товар</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>съестной припасы</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>бумажный товар</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>деревянный товар</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>крестьянский товар</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>москательный товар</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>мелкий товар</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>лавочный товар</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>рукоделие</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>шерстяной товар</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>красный товар</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>гарусный товар</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>мелочь</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>особливый товар</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>деревенский товар</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>серебреный товар</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>крамными товар</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>небогатый товар</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>мясо</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>железный товар</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>приуготовлять</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>набойчатый товар</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>щепетильный товар</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>пушной товар</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>нужный товар</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>внутренний товар</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>питейный припасы</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>недорогой товар</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>медный товар</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>привозный товар</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>оловянный товар</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>суровский товар</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>произрастание</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>галантерейный товар</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>купецкий товар</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>заморский товар</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>меховой товар</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>харчевой припасы</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>рукодельный товар</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>домовый товар</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>надлежащий товар</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
-                <c:pt idx="0">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="68075008"/>
-        <c:axId val="44394176"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="68075008"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44394176"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="44394176"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68075008"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -708,7 +291,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -743,7 +325,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -919,24 +500,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -944,7 +520,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -952,7 +528,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -960,7 +536,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -968,7 +544,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -976,7 +552,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -984,7 +560,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -992,7 +568,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1000,7 +576,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1008,7 +584,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1024,7 +600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1032,7 +608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1048,7 +624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1056,7 +632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1064,7 +640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1072,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1080,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1088,7 +664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1104,7 +680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1112,7 +688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1120,7 +696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1128,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1136,7 +712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1152,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1160,7 +736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1168,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1176,7 +752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1184,7 +760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1192,7 +768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1200,7 +776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1208,7 +784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1216,7 +792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1224,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1232,7 +808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1240,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1248,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1256,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1264,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1274,6 +850,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes from interrogating dataset for new patterns
Looked for entries that didn't currently have a fair associated with them, and exported to a csv for examination by longest descriptions. This has led to some additions to holiday regex. The goal now is to include weekly fairs, but not to include fairs that have no possibility of a defined temporal element.
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -64,72 +64,78 @@
     <t>мелочь</t>
   </si>
   <si>
+    <t>деревенский товар</t>
+  </si>
+  <si>
     <t>серебреный товар</t>
   </si>
   <si>
-    <t>деревенский товар</t>
-  </si>
-  <si>
     <t>небогатый товар</t>
   </si>
   <si>
     <t>крамными товар</t>
   </si>
   <si>
+    <t>железный товар</t>
+  </si>
+  <si>
     <t>мясо</t>
   </si>
   <si>
-    <t>железный товар</t>
-  </si>
-  <si>
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>щепетильный товар</t>
+  </si>
+  <si>
     <t>пушной товар</t>
   </si>
   <si>
+    <t>набойчатый товар</t>
+  </si>
+  <si>
     <t>нужный товар</t>
   </si>
   <si>
-    <t>набойчатый товар</t>
-  </si>
-  <si>
-    <t>щепетильный товар</t>
+    <t>питейный припасы</t>
+  </si>
+  <si>
+    <t>внутренний товар</t>
   </si>
   <si>
     <t>медный товар</t>
   </si>
   <si>
-    <t>питейный припасы</t>
-  </si>
-  <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
     <t>недорогой товар</t>
   </si>
   <si>
+    <t>оловянный товар</t>
+  </si>
+  <si>
     <t>привозный товар</t>
   </si>
   <si>
     <t>суровский товар</t>
   </si>
   <si>
-    <t>оловянный товар</t>
-  </si>
-  <si>
     <t>произрастание</t>
   </si>
   <si>
+    <t>заморский товар</t>
+  </si>
+  <si>
     <t>галантерейный товар</t>
   </si>
   <si>
-    <t>заморский товар</t>
-  </si>
-  <si>
     <t>купецкий товар</t>
   </si>
   <si>
+    <t>харчевой припасы</t>
+  </si>
+  <si>
+    <t>надлежащий товар</t>
+  </si>
+  <si>
     <t>меховой товар</t>
   </si>
   <si>
@@ -137,12 +143,6 @@
   </si>
   <si>
     <t>домовый товар</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
changes from re-running notebooks
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -58,91 +58,91 @@
     <t>гарусный товар</t>
   </si>
   <si>
+    <t>мелочь</t>
+  </si>
+  <si>
     <t>особливый товар</t>
   </si>
   <si>
-    <t>мелочь</t>
+    <t>серебреный товар</t>
   </si>
   <si>
     <t>деревенский товар</t>
   </si>
   <si>
-    <t>серебреный товар</t>
+    <t>небогатый товар</t>
   </si>
   <si>
     <t>крамными товар</t>
   </si>
   <si>
-    <t>небогатый товар</t>
+    <t>мясо</t>
   </si>
   <si>
     <t>железный товар</t>
   </si>
   <si>
-    <t>мясо</t>
-  </si>
-  <si>
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>щепетильный товар</t>
+  </si>
+  <si>
+    <t>пушной товар</t>
+  </si>
+  <si>
+    <t>набойчатый товар</t>
+  </si>
+  <si>
     <t>нужный товар</t>
   </si>
   <si>
-    <t>набойчатый товар</t>
-  </si>
-  <si>
-    <t>щепетильный товар</t>
-  </si>
-  <si>
-    <t>пушной товар</t>
-  </si>
-  <si>
     <t>недорогой товар</t>
   </si>
   <si>
+    <t>внутренний товар</t>
+  </si>
+  <si>
+    <t>питейный припасы</t>
+  </si>
+  <si>
     <t>суровский товар</t>
   </si>
   <si>
     <t>медный товар</t>
   </si>
   <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
-    <t>питейный припасы</t>
+    <t>привозный товар</t>
   </si>
   <si>
     <t>оловянный товар</t>
   </si>
   <si>
-    <t>привозный товар</t>
-  </si>
-  <si>
     <t>произрастание</t>
   </si>
   <si>
     <t>галантерейный товар</t>
   </si>
   <si>
+    <t>заморский товар</t>
+  </si>
+  <si>
     <t>купецкий товар</t>
   </si>
   <si>
-    <t>заморский товар</t>
+    <t>домовый товар</t>
+  </si>
+  <si>
+    <t>харчевой припасы</t>
   </si>
   <si>
     <t>меховой товар</t>
   </si>
   <si>
+    <t>рукодельный товар</t>
+  </si>
+  <si>
     <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>домовый товар</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
changes from adding re-running notebook on updated data.
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -64,12 +64,12 @@
     <t>особливый товар</t>
   </si>
   <si>
+    <t>деревенский товар</t>
+  </si>
+  <si>
     <t>серебреный товар</t>
   </si>
   <si>
-    <t>деревенский товар</t>
-  </si>
-  <si>
     <t>небогатый товар</t>
   </si>
   <si>
@@ -85,33 +85,33 @@
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>пушной товар</t>
+  </si>
+  <si>
+    <t>нужный товар</t>
+  </si>
+  <si>
+    <t>набойчатый товар</t>
+  </si>
+  <si>
     <t>щепетильный товар</t>
   </si>
   <si>
-    <t>пушной товар</t>
-  </si>
-  <si>
-    <t>набойчатый товар</t>
-  </si>
-  <si>
-    <t>нужный товар</t>
+    <t>питейный припасы</t>
+  </si>
+  <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
+    <t>медный товар</t>
+  </si>
+  <si>
+    <t>внутренний товар</t>
   </si>
   <si>
     <t>недорогой товар</t>
   </si>
   <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
-    <t>питейный припасы</t>
-  </si>
-  <si>
-    <t>суровский товар</t>
-  </si>
-  <si>
-    <t>медный товар</t>
-  </si>
-  <si>
     <t>привозный товар</t>
   </si>
   <si>
@@ -121,13 +121,16 @@
     <t>произрастание</t>
   </si>
   <si>
+    <t>купецкий товар</t>
+  </si>
+  <si>
+    <t>заморский товар</t>
+  </si>
+  <si>
     <t>галантерейный товар</t>
   </si>
   <si>
-    <t>заморский товар</t>
-  </si>
-  <si>
-    <t>купецкий товар</t>
+    <t>меховой товар</t>
   </si>
   <si>
     <t>домовый товар</t>
@@ -136,13 +139,10 @@
     <t>харчевой припасы</t>
   </si>
   <si>
-    <t>меховой товар</t>
+    <t>надлежащий товар</t>
   </si>
   <si>
     <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
made changes to handling of weekly fairs
Weekly fairs are now tracked, but not added to the dataset. They will likely be added at a later time under a different key, perhaps. Experimentation will be needed to find out the most useful way to interpret them
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -64,12 +64,12 @@
     <t>особливый товар</t>
   </si>
   <si>
+    <t>серебреный товар</t>
+  </si>
+  <si>
     <t>деревенский товар</t>
   </si>
   <si>
-    <t>серебреный товар</t>
-  </si>
-  <si>
     <t>небогатый товар</t>
   </si>
   <si>
@@ -88,55 +88,55 @@
     <t>пушной товар</t>
   </si>
   <si>
+    <t>набойчатый товар</t>
+  </si>
+  <si>
     <t>нужный товар</t>
   </si>
   <si>
-    <t>набойчатый товар</t>
-  </si>
-  <si>
     <t>щепетильный товар</t>
   </si>
   <si>
+    <t>недорогой товар</t>
+  </si>
+  <si>
+    <t>внутренний товар</t>
+  </si>
+  <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
+    <t>медный товар</t>
+  </si>
+  <si>
     <t>питейный припасы</t>
   </si>
   <si>
-    <t>суровский товар</t>
-  </si>
-  <si>
-    <t>медный товар</t>
-  </si>
-  <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
-    <t>недорогой товар</t>
+    <t>оловянный товар</t>
   </si>
   <si>
     <t>привозный товар</t>
   </si>
   <si>
-    <t>оловянный товар</t>
-  </si>
-  <si>
     <t>произрастание</t>
   </si>
   <si>
     <t>купецкий товар</t>
   </si>
   <si>
+    <t>галантерейный товар</t>
+  </si>
+  <si>
     <t>заморский товар</t>
   </si>
   <si>
-    <t>галантерейный товар</t>
+    <t>харчевой припасы</t>
   </si>
   <si>
     <t>меховой товар</t>
   </si>
   <si>
     <t>домовый товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
   </si>
   <si>
     <t>надлежащий товар</t>

</xml_diff>

<commit_message>
re-ran both text processing notebooks to re-generate dataset.
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -58,24 +58,24 @@
     <t>гарусный товар</t>
   </si>
   <si>
+    <t>особливый товар</t>
+  </si>
+  <si>
     <t>мелочь</t>
   </si>
   <si>
-    <t>особливый товар</t>
-  </si>
-  <si>
     <t>серебреный товар</t>
   </si>
   <si>
     <t>деревенский товар</t>
   </si>
   <si>
+    <t>крамными товар</t>
+  </si>
+  <si>
     <t>небогатый товар</t>
   </si>
   <si>
-    <t>крамными товар</t>
-  </si>
-  <si>
     <t>мясо</t>
   </si>
   <si>
@@ -85,64 +85,64 @@
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>щепетильный товар</t>
+  </si>
+  <si>
+    <t>нужный товар</t>
+  </si>
+  <si>
+    <t>набойчатый товар</t>
+  </si>
+  <si>
     <t>пушной товар</t>
   </si>
   <si>
-    <t>набойчатый товар</t>
-  </si>
-  <si>
-    <t>нужный товар</t>
-  </si>
-  <si>
-    <t>щепетильный товар</t>
+    <t>медный товар</t>
   </si>
   <si>
     <t>недорогой товар</t>
   </si>
   <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
+    <t>питейный припасы</t>
+  </si>
+  <si>
     <t>внутренний товар</t>
   </si>
   <si>
-    <t>суровский товар</t>
-  </si>
-  <si>
-    <t>медный товар</t>
-  </si>
-  <si>
-    <t>питейный припасы</t>
-  </si>
-  <si>
     <t>оловянный товар</t>
   </si>
   <si>
     <t>привозный товар</t>
   </si>
   <si>
+    <t>заморский товар</t>
+  </si>
+  <si>
+    <t>галантерейный товар</t>
+  </si>
+  <si>
     <t>произрастание</t>
   </si>
   <si>
     <t>купецкий товар</t>
   </si>
   <si>
-    <t>галантерейный товар</t>
-  </si>
-  <si>
-    <t>заморский товар</t>
+    <t>домовый товар</t>
   </si>
   <si>
     <t>харчевой припасы</t>
   </si>
   <si>
+    <t>рукодельный товар</t>
+  </si>
+  <si>
     <t>меховой товар</t>
   </si>
   <si>
-    <t>домовый товар</t>
-  </si>
-  <si>
     <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
changes from re-running adv text processing
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -70,12 +70,12 @@
     <t>деревенский товар</t>
   </si>
   <si>
+    <t>небогатый товар</t>
+  </si>
+  <si>
     <t>крамными товар</t>
   </si>
   <si>
-    <t>небогатый товар</t>
-  </si>
-  <si>
     <t>мясо</t>
   </si>
   <si>
@@ -97,52 +97,52 @@
     <t>пушной товар</t>
   </si>
   <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
+    <t>недорогой товар</t>
+  </si>
+  <si>
     <t>медный товар</t>
   </si>
   <si>
-    <t>недорогой товар</t>
-  </si>
-  <si>
-    <t>суровский товар</t>
+    <t>внутренний товар</t>
   </si>
   <si>
     <t>питейный припасы</t>
   </si>
   <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
     <t>оловянный товар</t>
   </si>
   <si>
     <t>привозный товар</t>
   </si>
   <si>
+    <t>произрастание</t>
+  </si>
+  <si>
+    <t>галантерейный товар</t>
+  </si>
+  <si>
+    <t>купецкий товар</t>
+  </si>
+  <si>
     <t>заморский товар</t>
   </si>
   <si>
-    <t>галантерейный товар</t>
-  </si>
-  <si>
-    <t>произрастание</t>
-  </si>
-  <si>
-    <t>купецкий товар</t>
+    <t>меховой товар</t>
+  </si>
+  <si>
+    <t>харчевой припасы</t>
+  </si>
+  <si>
+    <t>надлежащий товар</t>
+  </si>
+  <si>
+    <t>рукодельный товар</t>
   </si>
   <si>
     <t>домовый товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>меховой товар</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
re-ran text processing to re-generate geojson.
some files have changes just from re-ordering. the only significant changes are in the geojson file.
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -58,33 +58,36 @@
     <t>гарусный товар</t>
   </si>
   <si>
+    <t>мелочь</t>
+  </si>
+  <si>
     <t>особливый товар</t>
   </si>
   <si>
-    <t>мелочь</t>
+    <t>деревенский товар</t>
   </si>
   <si>
     <t>серебреный товар</t>
   </si>
   <si>
-    <t>деревенский товар</t>
+    <t>крамными товар</t>
   </si>
   <si>
     <t>небогатый товар</t>
   </si>
   <si>
-    <t>крамными товар</t>
+    <t>железный товар</t>
   </si>
   <si>
     <t>мясо</t>
   </si>
   <si>
-    <t>железный товар</t>
-  </si>
-  <si>
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>пушной товар</t>
+  </si>
+  <si>
     <t>щепетильный товар</t>
   </si>
   <si>
@@ -94,55 +97,52 @@
     <t>набойчатый товар</t>
   </si>
   <si>
-    <t>пушной товар</t>
-  </si>
-  <si>
     <t>суровский товар</t>
   </si>
   <si>
     <t>недорогой товар</t>
   </si>
   <si>
+    <t>внутренний товар</t>
+  </si>
+  <si>
+    <t>питейный припасы</t>
+  </si>
+  <si>
     <t>медный товар</t>
   </si>
   <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
-    <t>питейный припасы</t>
+    <t>привозный товар</t>
   </si>
   <si>
     <t>оловянный товар</t>
   </si>
   <si>
-    <t>привозный товар</t>
-  </si>
-  <si>
     <t>произрастание</t>
   </si>
   <si>
+    <t>заморский товар</t>
+  </si>
+  <si>
+    <t>купецкий товар</t>
+  </si>
+  <si>
     <t>галантерейный товар</t>
   </si>
   <si>
-    <t>купецкий товар</t>
-  </si>
-  <si>
-    <t>заморский товар</t>
+    <t>надлежащий товар</t>
+  </si>
+  <si>
+    <t>домовый товар</t>
+  </si>
+  <si>
+    <t>харчевой припасы</t>
+  </si>
+  <si>
+    <t>рукодельный товар</t>
   </si>
   <si>
     <t>меховой товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>домовый товар</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
reran script to re-process text after fixes
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -70,45 +70,45 @@
     <t>серебреный товар</t>
   </si>
   <si>
+    <t>небогатый товар</t>
+  </si>
+  <si>
     <t>крамными товар</t>
   </si>
   <si>
-    <t>небогатый товар</t>
+    <t>мясо</t>
   </si>
   <si>
     <t>железный товар</t>
   </si>
   <si>
-    <t>мясо</t>
-  </si>
-  <si>
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>набойчатый товар</t>
+  </si>
+  <si>
+    <t>щепетильный товар</t>
+  </si>
+  <si>
+    <t>нужный товар</t>
+  </si>
+  <si>
     <t>пушной товар</t>
   </si>
   <si>
-    <t>щепетильный товар</t>
-  </si>
-  <si>
-    <t>нужный товар</t>
-  </si>
-  <si>
-    <t>набойчатый товар</t>
+    <t>внутренний товар</t>
+  </si>
+  <si>
+    <t>недорогой товар</t>
+  </si>
+  <si>
+    <t>питейный припасы</t>
   </si>
   <si>
     <t>суровский товар</t>
   </si>
   <si>
-    <t>недорогой товар</t>
-  </si>
-  <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
-    <t>питейный припасы</t>
-  </si>
-  <si>
     <t>медный товар</t>
   </si>
   <si>
@@ -121,28 +121,28 @@
     <t>произрастание</t>
   </si>
   <si>
+    <t>купецкий товар</t>
+  </si>
+  <si>
+    <t>галантерейный товар</t>
+  </si>
+  <si>
     <t>заморский товар</t>
   </si>
   <si>
-    <t>купецкий товар</t>
-  </si>
-  <si>
-    <t>галантерейный товар</t>
+    <t>меховой товар</t>
+  </si>
+  <si>
+    <t>рукодельный товар</t>
+  </si>
+  <si>
+    <t>домовый товар</t>
   </si>
   <si>
     <t>надлежащий товар</t>
   </si>
   <si>
-    <t>домовый товар</t>
-  </si>
-  <si>
     <t>харчевой припасы</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>меховой товар</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
reran both text processing in preparation for new round of geocoding
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -58,24 +58,24 @@
     <t>гарусный товар</t>
   </si>
   <si>
+    <t>особливый товар</t>
+  </si>
+  <si>
     <t>мелочь</t>
   </si>
   <si>
-    <t>особливый товар</t>
-  </si>
-  <si>
     <t>деревенский товар</t>
   </si>
   <si>
     <t>серебреный товар</t>
   </si>
   <si>
+    <t>крамными товар</t>
+  </si>
+  <si>
     <t>небогатый товар</t>
   </si>
   <si>
-    <t>крамными товар</t>
-  </si>
-  <si>
     <t>мясо</t>
   </si>
   <si>
@@ -85,49 +85,55 @@
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>щепетильный товар</t>
+  </si>
+  <si>
+    <t>пушной товар</t>
+  </si>
+  <si>
+    <t>нужный товар</t>
+  </si>
+  <si>
     <t>набойчатый товар</t>
   </si>
   <si>
-    <t>щепетильный товар</t>
-  </si>
-  <si>
-    <t>нужный товар</t>
-  </si>
-  <si>
-    <t>пушной товар</t>
+    <t>медный товар</t>
+  </si>
+  <si>
+    <t>недорогой товар</t>
   </si>
   <si>
     <t>внутренний товар</t>
   </si>
   <si>
-    <t>недорогой товар</t>
-  </si>
-  <si>
     <t>питейный припасы</t>
   </si>
   <si>
     <t>суровский товар</t>
   </si>
   <si>
-    <t>медный товар</t>
+    <t>оловянный товар</t>
   </si>
   <si>
     <t>привозный товар</t>
   </si>
   <si>
-    <t>оловянный товар</t>
+    <t>купецкий товар</t>
+  </si>
+  <si>
+    <t>заморский товар</t>
   </si>
   <si>
     <t>произрастание</t>
   </si>
   <si>
-    <t>купецкий товар</t>
-  </si>
-  <si>
     <t>галантерейный товар</t>
   </si>
   <si>
-    <t>заморский товар</t>
+    <t>надлежащий товар</t>
+  </si>
+  <si>
+    <t>харчевой припасы</t>
   </si>
   <si>
     <t>меховой товар</t>
@@ -137,12 +143,6 @@
   </si>
   <si>
     <t>домовый товар</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
replaced variable names. see previous commit for specifics
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -70,12 +70,12 @@
     <t>деревенский товар</t>
   </si>
   <si>
+    <t>крамными товар</t>
+  </si>
+  <si>
     <t>небогатый товар</t>
   </si>
   <si>
-    <t>крамными товар</t>
-  </si>
-  <si>
     <t>железный товар</t>
   </si>
   <si>
@@ -85,33 +85,33 @@
     <t>приуготовлять</t>
   </si>
   <si>
+    <t>нужный товар</t>
+  </si>
+  <si>
+    <t>пушной товар</t>
+  </si>
+  <si>
+    <t>щепетильный товар</t>
+  </si>
+  <si>
     <t>набойчатый товар</t>
   </si>
   <si>
-    <t>нужный товар</t>
-  </si>
-  <si>
-    <t>щепетильный товар</t>
-  </si>
-  <si>
-    <t>пушной товар</t>
+    <t>медный товар</t>
   </si>
   <si>
     <t>суровский товар</t>
   </si>
   <si>
+    <t>питейный припасы</t>
+  </si>
+  <si>
+    <t>внутренний товар</t>
+  </si>
+  <si>
     <t>недорогой товар</t>
   </si>
   <si>
-    <t>медный товар</t>
-  </si>
-  <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
-    <t>питейный припасы</t>
-  </si>
-  <si>
     <t>оловянный товар</t>
   </si>
   <si>
@@ -121,28 +121,28 @@
     <t>галантерейный товар</t>
   </si>
   <si>
+    <t>произрастание</t>
+  </si>
+  <si>
+    <t>купецкий товар</t>
+  </si>
+  <si>
     <t>заморский товар</t>
   </si>
   <si>
-    <t>произрастание</t>
-  </si>
-  <si>
-    <t>купецкий товар</t>
+    <t>меховой товар</t>
+  </si>
+  <si>
+    <t>харчевой припасы</t>
+  </si>
+  <si>
+    <t>надлежащий товар</t>
+  </si>
+  <si>
+    <t>рукодельный товар</t>
   </si>
   <si>
     <t>домовый товар</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
-  </si>
-  <si>
-    <t>меховой товар</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
re-generated goods export with fillna(0)
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -58,64 +58,67 @@
     <t>гарусный товар</t>
   </si>
   <si>
+    <t>особливый товар</t>
+  </si>
+  <si>
     <t>мелочь</t>
   </si>
   <si>
-    <t>особливый товар</t>
+    <t>деревенский товар</t>
   </si>
   <si>
     <t>серебреный товар</t>
   </si>
   <si>
-    <t>деревенский товар</t>
+    <t>небогатый товар</t>
   </si>
   <si>
     <t>крамными товар</t>
   </si>
   <si>
-    <t>небогатый товар</t>
+    <t>мясо</t>
   </si>
   <si>
     <t>железный товар</t>
   </si>
   <si>
-    <t>мясо</t>
-  </si>
-  <si>
     <t>приуготовлять</t>
   </si>
   <si>
     <t>нужный товар</t>
   </si>
   <si>
+    <t>щепетильный товар</t>
+  </si>
+  <si>
     <t>пушной товар</t>
   </si>
   <si>
-    <t>щепетильный товар</t>
-  </si>
-  <si>
     <t>набойчатый товар</t>
   </si>
   <si>
+    <t>недорогой товар</t>
+  </si>
+  <si>
+    <t>питейный припасы</t>
+  </si>
+  <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
     <t>медный товар</t>
   </si>
   <si>
-    <t>суровский товар</t>
-  </si>
-  <si>
-    <t>питейный припасы</t>
-  </si>
-  <si>
     <t>внутренний товар</t>
   </si>
   <si>
-    <t>недорогой товар</t>
+    <t>привозный товар</t>
   </si>
   <si>
     <t>оловянный товар</t>
   </si>
   <si>
-    <t>привозный товар</t>
+    <t>купецкий товар</t>
   </si>
   <si>
     <t>галантерейный товар</t>
@@ -124,25 +127,22 @@
     <t>произрастание</t>
   </si>
   <si>
-    <t>купецкий товар</t>
-  </si>
-  <si>
     <t>заморский товар</t>
   </si>
   <si>
+    <t>домовый товар</t>
+  </si>
+  <si>
+    <t>надлежащий товар</t>
+  </si>
+  <si>
+    <t>рукодельный товар</t>
+  </si>
+  <si>
+    <t>харчевой припасы</t>
+  </si>
+  <si>
     <t>меховой товар</t>
-  </si>
-  <si>
-    <t>харчевой припасы</t>
-  </si>
-  <si>
-    <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>домовый товар</t>
   </si>
 </sst>
 </file>

</xml_diff>